<commit_message>
Updating all files. I've started adding a motor driver (vibration motor).
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -65,9 +65,6 @@
     <t>768-1129-1-ND</t>
   </si>
   <si>
-    <t>ATMEGA328P-15AZCT-ND</t>
-  </si>
-  <si>
     <t>MMA8452QT-ND</t>
   </si>
   <si>
@@ -78,6 +75,9 @@
   </si>
   <si>
     <t>PCB</t>
+  </si>
+  <si>
+    <t>ATMEGA328P-AU-ND</t>
   </si>
 </sst>
 </file>
@@ -395,7 +395,7 @@
   <dimension ref="B7:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -409,7 +409,7 @@
         <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D7">
         <v>6.71</v>
@@ -442,7 +442,7 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D10">
         <v>3.98</v>
@@ -453,7 +453,7 @@
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D11">
         <v>1.98</v>
@@ -492,7 +492,7 @@
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.2">
@@ -506,7 +506,7 @@
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D17">
         <v>7</v>

</xml_diff>